<commit_message>
project file and data
</commit_message>
<xml_diff>
--- a/NBASEASONSUMMARY/NBA2010-2011.xlsx
+++ b/NBASEASONSUMMARY/NBA2010-2011.xlsx
@@ -524,7 +524,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1">
@@ -607,7 +607,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1">
@@ -690,7 +690,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1">
@@ -773,7 +773,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
@@ -856,7 +856,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="1">
@@ -939,7 +939,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="1">
@@ -1022,7 +1022,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1">
@@ -1105,7 +1105,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="1">
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="1">
@@ -1271,7 +1271,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="1">
@@ -1354,7 +1354,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1">
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="1">
@@ -1520,7 +1520,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="1">
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="1">
@@ -1686,7 +1686,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="1">
@@ -1769,7 +1769,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1">
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="1">
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="1">
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="1">
@@ -2101,7 +2101,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="1">
@@ -2184,7 +2184,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="1">
@@ -2267,7 +2267,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="1">
@@ -2350,7 +2350,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="1">
@@ -2433,7 +2433,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="1">
@@ -2516,7 +2516,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="1">
@@ -2599,7 +2599,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="1">
@@ -2682,7 +2682,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="1">
@@ -2765,7 +2765,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="1">
@@ -2848,7 +2848,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B30" s="1">
@@ -2931,7 +2931,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="1">

</xml_diff>